<commit_message>
MW to MWh correction
</commit_message>
<xml_diff>
--- a/Output/Tables/table 3 - fuel type 2018 stats.xlsx
+++ b/Output/Tables/table 3 - fuel type 2018 stats.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7300"/>
   </bookViews>
   <sheets>
     <sheet name="fuel type 2018 stats" sheetId="1" r:id="rId1"/>
@@ -67,10 +67,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="165" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,15 +202,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -558,8 +550,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -881,38 +873,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="A1:F9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -920,160 +910,170 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2">
-        <v>13085.946099999999</v>
-      </c>
-      <c r="C2" s="2">
-        <v>-485.323913251899</v>
-      </c>
-      <c r="D2" s="2">
-        <v>-376.323109961108</v>
+      <c r="B2" s="1">
+        <v>1.08240472833333</v>
+      </c>
+      <c r="C2" s="1">
+        <v>550.96574363693298</v>
+      </c>
+      <c r="D2" s="1">
+        <v>416.16601062843699</v>
       </c>
       <c r="E2" s="2">
-        <v>-6350922.5698554302</v>
+        <v>0.59636792606230693</v>
       </c>
       <c r="F2" s="2">
-        <v>-4924543.9331354303</v>
+        <v>0.45046005767583996</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2">
-        <v>4642198.91151</v>
-      </c>
-      <c r="C3" s="2">
-        <v>-22.3935741105925</v>
-      </c>
-      <c r="D3" s="2">
-        <v>-16.247083499126099</v>
-      </c>
-      <c r="E3" s="2">
-        <v>-103955425.361011</v>
-      </c>
-      <c r="F3" s="2">
-        <v>-75422193.334855095</v>
+      <c r="B3" s="1">
+        <v>388.038161020833</v>
+      </c>
+      <c r="C3" s="1">
+        <v>22.6838772985903</v>
+      </c>
+      <c r="D3" s="1">
+        <v>16.377724522323899</v>
+      </c>
+      <c r="E3" s="1">
+        <v>8.8022100317672098</v>
+      </c>
+      <c r="F3" s="1">
+        <v>6.3551821053483595</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2">
-        <v>18609239.286049999</v>
-      </c>
-      <c r="C4" s="2">
-        <v>-10.9162496936962</v>
-      </c>
-      <c r="D4" s="2">
-        <v>-8.25357628271518</v>
-      </c>
-      <c r="E4" s="2">
-        <v>-203143102.65626201</v>
-      </c>
-      <c r="F4" s="2">
-        <v>-153592776.01071399</v>
+      <c r="B4" s="1">
+        <v>1551.00895077833</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10.9604839706953</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8.2663260448639608</v>
+      </c>
+      <c r="E4" s="1">
+        <v>16.999808743410799</v>
+      </c>
+      <c r="F4" s="1">
+        <v>12.821145685636099</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2">
-        <v>866970.17631000001</v>
-      </c>
-      <c r="C5" s="2">
-        <v>-95.359017666655305</v>
-      </c>
-      <c r="D5" s="2">
-        <v>-49.695424977782402</v>
-      </c>
-      <c r="E5" s="2">
-        <v>-82673424.359208494</v>
-      </c>
-      <c r="F5" s="2">
-        <v>-43084451.354788303</v>
+      <c r="B5" s="1">
+        <v>71.982325360000004</v>
+      </c>
+      <c r="C5" s="1">
+        <v>97.219670258001699</v>
+      </c>
+      <c r="D5" s="1">
+        <v>49.959810688289799</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6.9980979359034006</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3.59622334788848</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2">
-        <v>12429658.629410001</v>
-      </c>
-      <c r="C6" s="2">
-        <v>-80.713069442178707</v>
-      </c>
-      <c r="D6" s="2">
-        <v>-73.529249010676395</v>
-      </c>
-      <c r="E6" s="2">
-        <v>-1003235900.09815</v>
-      </c>
-      <c r="F6" s="2">
-        <v>-913943464.47959101</v>
+      <c r="B6" s="1">
+        <v>1032.84026755083</v>
+      </c>
+      <c r="C6" s="1">
+        <v>81.954842242142107</v>
+      </c>
+      <c r="D6" s="1">
+        <v>74.477724496221001</v>
+      </c>
+      <c r="E6" s="1">
+        <v>84.646261188460301</v>
+      </c>
+      <c r="F6" s="1">
+        <v>76.923592895254103</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2">
-        <v>15132.155430000001</v>
-      </c>
-      <c r="C7" s="2">
-        <v>-560.12457000279903</v>
-      </c>
-      <c r="D7" s="2">
-        <v>-144.353233644222</v>
-      </c>
-      <c r="E7" s="2">
-        <v>-8475892.05344427</v>
-      </c>
-      <c r="F7" s="2">
-        <v>-2184375.5683274702</v>
+      <c r="B7" s="1">
+        <v>1.2871983091666701</v>
+      </c>
+      <c r="C7" s="1">
+        <v>884.29563198907294</v>
+      </c>
+      <c r="D7" s="1">
+        <v>439.70755741240498</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.1382638422997999</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.56599082442905302</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2">
-        <v>687197.21617000003</v>
-      </c>
-      <c r="C8" s="2">
-        <v>-83.261831819322893</v>
-      </c>
-      <c r="D8" s="2">
-        <v>88.879441105251402</v>
-      </c>
-      <c r="E8" s="2">
-        <v>-57217299.039453402</v>
-      </c>
-      <c r="F8" s="2">
-        <v>61077704.5022742</v>
+      <c r="B8" s="1">
+        <v>56.044908320000005</v>
+      </c>
+      <c r="C8" s="1">
+        <v>71.834835441691197</v>
+      </c>
+      <c r="D8" s="1">
+        <v>-93.892694186698094</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4.02597676651187</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-5.2622074376112904</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2">
-        <v>21274370.981860001</v>
-      </c>
-      <c r="C9" s="2">
-        <v>-667.43439033964705</v>
-      </c>
-      <c r="D9" s="2">
-        <v>-28.673951377895101</v>
-      </c>
-      <c r="E9" s="2">
-        <v>-14199246826.137199</v>
-      </c>
-      <c r="F9" s="2">
-        <v>-610020279.12915504</v>
+      <c r="B9" s="1">
+        <v>1760.0948655091702</v>
+      </c>
+      <c r="C9" s="1">
+        <v>669.35195732655097</v>
+      </c>
+      <c r="D9" s="1">
+        <v>29.255740162575801</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1178.12294330897</v>
+      </c>
+      <c r="F9" s="1">
+        <v>51.492878046819904</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E10" s="2">
+        <f>SUM(E2:E9)</f>
+        <v>1301.3299297433857</v>
+      </c>
+      <c r="F10" s="2">
+        <f>SUM(F2:F9)</f>
+        <v>146.94326552544055</v>
       </c>
     </row>
   </sheetData>

</xml_diff>